<commit_message>
Complete logs for 13 week
</commit_message>
<xml_diff>
--- a/Logs/13th Week TeamLogs.xlsx
+++ b/Logs/13th Week TeamLogs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0B4640-D809-4B36-981D-1ED642FF8A99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D778F2-3E8C-4A2B-9F50-8F1A3DBB50D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jegor" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -89,14 +88,33 @@
   </si>
   <si>
     <t>DesingPattern</t>
+  </si>
+  <si>
+    <t>Prog.</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Praktikum</t>
+  </si>
+  <si>
+    <t>Remakeing whole project</t>
+  </si>
+  <si>
+    <t>Mustrid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -186,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -520,11 +538,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -587,14 +625,11 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -621,13 +656,32 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -914,19 +968,18 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="37.44140625" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="37.42578125" customWidth="1"/>
+    <col min="10" max="11" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>11</v>
       </c>
@@ -940,7 +993,7 @@
       <c r="J3" s="23"/>
       <c r="K3" s="24"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="25"/>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
@@ -952,7 +1005,7 @@
       <c r="J4" s="26"/>
       <c r="K4" s="27"/>
     </row>
-    <row r="5" spans="2:11" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>10</v>
       </c>
@@ -970,7 +1023,7 @@
       <c r="J5" s="33"/>
       <c r="K5" s="34"/>
     </row>
-    <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -982,7 +1035,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="2:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
@@ -1012,24 +1065,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="65">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="62">
         <v>1</v>
       </c>
-      <c r="C8" s="66">
+      <c r="C8" s="63">
         <v>43577</v>
       </c>
-      <c r="D8" s="67">
+      <c r="D8" s="64">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E8" s="67">
+      <c r="E8" s="64">
         <v>0.72916666666666663</v>
       </c>
-      <c r="F8" s="59"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="11">
         <v>330</v>
       </c>
-      <c r="H8" s="62" t="s">
+      <c r="H8" s="59" t="s">
         <v>17</v>
       </c>
       <c r="I8" s="20" t="s">
@@ -1038,24 +1091,24 @@
       <c r="J8" s="7"/>
       <c r="K8" s="37"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="65">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="62">
         <v>2</v>
       </c>
-      <c r="C9" s="63">
+      <c r="C9" s="60">
         <v>43580</v>
       </c>
-      <c r="D9" s="80">
+      <c r="D9" s="75">
         <v>0.5</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="61">
         <v>0.95138888888888884</v>
       </c>
-      <c r="F9" s="60"/>
+      <c r="F9" s="57"/>
       <c r="G9" s="11">
         <v>510</v>
       </c>
-      <c r="H9" s="70" t="s">
+      <c r="H9" s="67" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="20" t="s">
@@ -1064,24 +1117,24 @@
       <c r="J9" s="4"/>
       <c r="K9" s="38"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="65">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="62">
         <v>3</v>
       </c>
-      <c r="C10" s="63">
+      <c r="C10" s="60">
         <v>43581</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="61">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="61">
         <v>0.95833333333333337</v>
       </c>
-      <c r="F10" s="60"/>
+      <c r="F10" s="57"/>
       <c r="G10" s="11">
         <v>180</v>
       </c>
-      <c r="H10" s="70" t="s">
+      <c r="H10" s="67" t="s">
         <v>17</v>
       </c>
       <c r="I10" s="20" t="s">
@@ -1090,45 +1143,45 @@
       <c r="J10" s="4"/>
       <c r="K10" s="38"/>
     </row>
-    <row r="11" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="65"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="60"/>
+    <row r="11" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="62"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="57"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="62"/>
+      <c r="H11" s="59"/>
       <c r="I11" s="20"/>
       <c r="J11" s="4"/>
       <c r="K11" s="38"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="65"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="62"/>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="62"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="59"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="62"/>
+      <c r="H12" s="59"/>
       <c r="I12" s="20"/>
       <c r="J12" s="4"/>
       <c r="K12" s="38"/>
     </row>
-    <row r="13" spans="2:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="65"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="62"/>
+    <row r="13" spans="2:11" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="62"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="59"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="62"/>
+      <c r="H13" s="59"/>
       <c r="I13" s="20"/>
       <c r="J13" s="4"/>
       <c r="K13" s="38"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
-      <c r="C14" s="45"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
       <c r="F14" s="40"/>
@@ -1138,9 +1191,9 @@
       <c r="J14" s="4"/>
       <c r="K14" s="38"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
-      <c r="C15" s="45"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
       <c r="F15" s="40"/>
@@ -1150,7 +1203,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="38"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="35"/>
       <c r="C16" s="5"/>
       <c r="D16" s="13"/>
@@ -1162,7 +1215,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="38"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="35"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1174,7 +1227,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="38"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="35"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1186,7 +1239,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="38"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="35"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1198,7 +1251,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="38"/>
     </row>
-    <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="36"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -1210,7 +1263,7 @@
       <c r="J20" s="6"/>
       <c r="K20" s="39"/>
     </row>
-    <row r="21" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -1241,17 +1294,17 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>11</v>
       </c>
@@ -1265,7 +1318,7 @@
       <c r="J4" s="23"/>
       <c r="K4" s="24"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
@@ -1277,7 +1330,7 @@
       <c r="J5" s="26"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="28" t="s">
         <v>10</v>
       </c>
@@ -1290,12 +1343,14 @@
       <c r="G6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="32"/>
+      <c r="H6" s="83">
+        <v>43577</v>
+      </c>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1307,11 +1362,11 @@
       <c r="J7" s="2"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="2:11" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="78" t="s">
+    <row r="8" spans="2:11" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
@@ -1337,81 +1392,156 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="68"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="44"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="68"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="43"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="68"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="43"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="68"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="43"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="68"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="43"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="68"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="62"/>
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="71">
+        <v>1</v>
+      </c>
+      <c r="C9" s="72">
+        <v>43577</v>
+      </c>
+      <c r="D9" s="73">
+        <v>0.875</v>
+      </c>
+      <c r="E9" s="73">
+        <v>1</v>
+      </c>
+      <c r="F9" s="74"/>
+      <c r="G9" s="78">
+        <f>(E9-D9)*24*60 - F9</f>
+        <v>180</v>
+      </c>
+      <c r="H9" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="74"/>
+      <c r="K9" s="48"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="70">
+        <v>2</v>
+      </c>
+      <c r="C10" s="68">
+        <v>43579</v>
+      </c>
+      <c r="D10" s="69">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E10" s="69">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F10" s="67"/>
+      <c r="G10" s="79">
+        <f t="shared" ref="G10:G13" si="0">(E10-D10)*24*60 - F10</f>
+        <v>180</v>
+      </c>
+      <c r="H10" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="67"/>
+      <c r="K10" s="47"/>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="70">
+        <v>3</v>
+      </c>
+      <c r="C11" s="68">
+        <v>43580</v>
+      </c>
+      <c r="D11" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="E11" s="69">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F11" s="67"/>
+      <c r="G11" s="79">
+        <f t="shared" si="0"/>
+        <v>300.00000000000006</v>
+      </c>
+      <c r="H11" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="67"/>
+      <c r="K11" s="47"/>
+    </row>
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="58">
+        <v>4</v>
+      </c>
+      <c r="C12" s="80">
+        <v>43581</v>
+      </c>
+      <c r="D12" s="81">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E12" s="81">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F12" s="82"/>
+      <c r="G12" s="79">
+        <f t="shared" si="0"/>
+        <v>270.00000000000011</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="67"/>
+      <c r="K12" s="47"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="58">
+        <v>5</v>
+      </c>
+      <c r="C13" s="80">
+        <v>43582</v>
+      </c>
+      <c r="D13" s="81">
+        <v>0.625</v>
+      </c>
+      <c r="E13" s="81">
+        <v>0.75</v>
+      </c>
+      <c r="F13" s="82"/>
+      <c r="G13" s="79">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="H13" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="67"/>
+      <c r="K13" s="47"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="65"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="59"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="68"/>
+      <c r="H14" s="65"/>
       <c r="I14" s="20"/>
       <c r="J14" s="40"/>
       <c r="K14" s="43"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
-      <c r="C15" s="45"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
       <c r="F15" s="40"/>
@@ -1421,9 +1551,9 @@
       <c r="J15" s="40"/>
       <c r="K15" s="43"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="42"/>
-      <c r="C16" s="45"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
       <c r="F16" s="40"/>
@@ -1433,9 +1563,9 @@
       <c r="J16" s="40"/>
       <c r="K16" s="43"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
-      <c r="C17" s="45"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="41"/>
       <c r="E17" s="41"/>
       <c r="F17" s="40"/>
@@ -1445,7 +1575,7 @@
       <c r="J17" s="40"/>
       <c r="K17" s="43"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="42"/>
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
@@ -1457,7 +1587,7 @@
       <c r="J18" s="40"/>
       <c r="K18" s="43"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="42"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
@@ -1469,7 +1599,7 @@
       <c r="J19" s="40"/>
       <c r="K19" s="43"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="42"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
@@ -1481,19 +1611,19 @@
       <c r="J20" s="40"/>
       <c r="K20" s="43"/>
     </row>
-    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="36"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="46"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="21"/>
-      <c r="J21" s="46"/>
+      <c r="J21" s="45"/>
       <c r="K21" s="39"/>
     </row>
-    <row r="22" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -1503,7 +1633,7 @@
       </c>
       <c r="G22" s="17">
         <f>SUM(G9:G21)</f>
-        <v>0</v>
+        <v>1110</v>
       </c>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
@@ -1522,22 +1652,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32427AFA-22DC-4EF4-A25E-0E66666CECD2}">
   <dimension ref="B3:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>11</v>
       </c>
@@ -1551,7 +1681,7 @@
       <c r="J4" s="23"/>
       <c r="K4" s="24"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
@@ -1563,7 +1693,7 @@
       <c r="J5" s="26"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="28" t="s">
         <v>10</v>
       </c>
@@ -1576,12 +1706,14 @@
       <c r="G6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="32"/>
+      <c r="H6" s="83">
+        <v>43577</v>
+      </c>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1593,11 +1725,11 @@
       <c r="J7" s="2"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="2:11" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="78" t="s">
+    <row r="8" spans="2:11" ht="34.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
@@ -1623,115 +1755,190 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="74"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="50"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="73"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="73"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="73"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="48"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="73"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="48"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="73"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="70"/>
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="71">
+        <v>1</v>
+      </c>
+      <c r="C9" s="72">
+        <v>43577</v>
+      </c>
+      <c r="D9" s="73">
+        <v>0.875</v>
+      </c>
+      <c r="E9" s="73">
+        <v>1</v>
+      </c>
+      <c r="F9" s="74"/>
+      <c r="G9" s="78">
+        <f>(E9-D9)*24*60 - F9</f>
+        <v>180</v>
+      </c>
+      <c r="H9" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="74"/>
+      <c r="K9" s="48"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="70">
+        <v>2</v>
+      </c>
+      <c r="C10" s="68">
+        <v>43578</v>
+      </c>
+      <c r="D10" s="69">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E10" s="69">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F10" s="67"/>
+      <c r="G10" s="79">
+        <f t="shared" ref="G10:G13" si="0">(E10-D10)*24*60 - F10</f>
+        <v>360</v>
+      </c>
+      <c r="H10" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="55"/>
+      <c r="K10" s="49"/>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="70">
+        <v>3</v>
+      </c>
+      <c r="C11" s="68">
+        <v>43579</v>
+      </c>
+      <c r="D11" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="E11" s="69">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F11" s="67"/>
+      <c r="G11" s="79">
+        <f t="shared" si="0"/>
+        <v>239.99999999999994</v>
+      </c>
+      <c r="H11" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="67"/>
+      <c r="K11" s="47"/>
+    </row>
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="71">
+        <v>4</v>
+      </c>
+      <c r="C12" s="68">
+        <v>43580</v>
+      </c>
+      <c r="D12" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="E12" s="69">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F12" s="67"/>
+      <c r="G12" s="79">
+        <f t="shared" si="0"/>
+        <v>300.00000000000006</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="67"/>
+      <c r="K12" s="47"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="70">
+        <v>5</v>
+      </c>
+      <c r="C13" s="80">
+        <v>43581</v>
+      </c>
+      <c r="D13" s="81">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E13" s="81">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F13" s="82"/>
+      <c r="G13" s="79">
+        <f t="shared" si="0"/>
+        <v>270.00000000000011</v>
+      </c>
+      <c r="H13" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="67"/>
+      <c r="K13" s="47"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="70"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="67"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="70"/>
+      <c r="H14" s="67"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="48"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="73"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="70"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="70"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="67"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="70"/>
+      <c r="H15" s="67"/>
       <c r="I15" s="19"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="48"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="73"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="70"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="70"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="67"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="70"/>
+      <c r="H16" s="67"/>
       <c r="I16" s="19"/>
       <c r="J16" s="4"/>
       <c r="K16" s="38"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="73"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="70"/>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="70"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="70"/>
+      <c r="H17" s="67"/>
       <c r="I17" s="19"/>
       <c r="J17" s="4"/>
       <c r="K17" s="38"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="35"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1743,7 +1950,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="38"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="35"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1755,7 +1962,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="38"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="35"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1767,7 +1974,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="38"/>
     </row>
-    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="36"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1779,7 +1986,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="39"/>
     </row>
-    <row r="22" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -1789,7 +1996,7 @@
       </c>
       <c r="G22" s="17">
         <f>SUM(G9:G21)</f>
-        <v>0</v>
+        <v>1350</v>
       </c>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
@@ -1806,24 +2013,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F48D277-4C33-425C-A628-D76A08925D5B}">
-  <dimension ref="B3:K22"/>
+  <dimension ref="B3:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
-    <col min="9" max="9" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>11</v>
       </c>
@@ -1837,7 +2044,7 @@
       <c r="J4" s="23"/>
       <c r="K4" s="24"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
@@ -1849,7 +2056,7 @@
       <c r="J5" s="26"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="28" t="s">
         <v>10</v>
       </c>
@@ -1862,12 +2069,14 @@
       <c r="G6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="32"/>
+      <c r="H6" s="83">
+        <v>43577</v>
+      </c>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1879,11 +2088,11 @@
       <c r="J7" s="2"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="2:11" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="78" t="s">
+    <row r="8" spans="2:11" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
@@ -1909,178 +2118,182 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="65"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="53"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="65"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="53"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="65"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="61"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="62"/>
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="87">
+        <v>1</v>
+      </c>
+      <c r="C9" s="96">
+        <v>43577</v>
+      </c>
+      <c r="D9" s="95">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E9" s="85">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F9" s="92"/>
+      <c r="G9" s="89">
+        <v>329.99999999999994</v>
+      </c>
+      <c r="H9" s="89" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="54"/>
+      <c r="K9" s="50"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="87">
+        <v>3</v>
+      </c>
+      <c r="C10" s="84">
+        <v>43580</v>
+      </c>
+      <c r="D10" s="85">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="88">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="F10" s="93">
+        <v>140</v>
+      </c>
+      <c r="G10" s="89">
+        <v>509.99999999999989</v>
+      </c>
+      <c r="H10" s="89"/>
+      <c r="I10" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="94">
+        <v>7</v>
+      </c>
+      <c r="C11" s="90">
+        <v>43581</v>
+      </c>
+      <c r="D11" s="88">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E11" s="88">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89">
+        <v>180</v>
+      </c>
+      <c r="H11" s="89"/>
+      <c r="I11" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="53"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="57"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="62"/>
+      <c r="H12" s="50"/>
       <c r="I12" s="19"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="65"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="60"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="53"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="50"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="62"/>
+      <c r="H13" s="50"/>
       <c r="I13" s="19"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="65"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="62"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="53"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="62"/>
+      <c r="H14" s="50"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="56"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="60"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="53"/>
+      <c r="H15" s="4"/>
       <c r="I15" s="19"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="56"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="53"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="56"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="53"/>
+      <c r="H17" s="4"/>
       <c r="I17" s="19"/>
       <c r="J17" s="4"/>
       <c r="K17" s="38"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="35"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="38"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="35"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="38"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="35"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="38"/>
-    </row>
-    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="36"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="39"/>
-    </row>
-    <row r="22" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16" t="s">
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="36"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="39"/>
+    </row>
+    <row r="19" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="17">
-        <f>SUM(G9:G21)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="18"/>
+      <c r="G19" s="17">
+        <f>SUM(G9:G18)</f>
+        <v>1019.9999999999998</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>